<commit_message>
Release Production V9: Intelligent Contact Filter & Auto-Setup
</commit_message>
<xml_diff>
--- a/data/contacts.xlsx
+++ b/data/contacts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>Interes</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Mensaje</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -473,30 +478,52 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Gabriel</t>
-        </is>
-      </c>
+      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>522205511054</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
+          <t>3339563030</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Prueba Cliente</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>522205511054</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Cita Agendada</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Hola Prueba Cliente, confirmamos tu cita para mañana a las 10:00. 🗓️ ¿Podrías confirmar con un 'SÍ'?</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>